<commit_message>
Add more tests & include testing setups
</commit_message>
<xml_diff>
--- a/Charts.xlsx
+++ b/Charts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\akdum\Downloads\GitHub\minecraft-server-hosts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C010430-03FF-4A39-BAB0-88404C08C3F9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BB82B02-74C6-4443-A4D2-B51B33F5F422}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{44A97144-5CF4-493B-8574-0BA792057902}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="29">
   <si>
     <t>Plan</t>
   </si>
@@ -182,567 +182,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:barChart>
-        <c:barDir val="bar"/>
-        <c:grouping val="clustered"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$B$2</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Score</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent1"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:dLbls>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-                <a:spAutoFit/>
-              </a:bodyPr>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="75000"/>
-                        <a:lumOff val="25000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:endParaRPr lang="en-US"/>
-              </a:p>
-            </c:txPr>
-            <c:dLblPos val="outEnd"/>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="1"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showBubbleSize val="0"/>
-            <c:showLeaderLines val="0"/>
-            <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:showLeaderLines val="1"/>
-                <c15:leaderLines>
-                  <c:spPr>
-                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="35000"/>
-                          <a:lumOff val="65000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:round/>
-                    </a:ln>
-                    <a:effectLst/>
-                  </c:spPr>
-                </c15:leaderLines>
-              </c:ext>
-            </c:extLst>
-          </c:dLbls>
-          <c:errBars>
-            <c:errBarType val="both"/>
-            <c:errValType val="cust"/>
-            <c:noEndCap val="0"/>
-            <c:plus>
-              <c:numRef>
-                <c:f>Sheet1!$C$3:$C$19</c:f>
-                <c:numCache>
-                  <c:formatCode>General</c:formatCode>
-                  <c:ptCount val="17"/>
-                  <c:pt idx="0">
-                    <c:v>4.0599999999999996</c:v>
-                  </c:pt>
-                  <c:pt idx="1">
-                    <c:v>0</c:v>
-                  </c:pt>
-                  <c:pt idx="2">
-                    <c:v>0</c:v>
-                  </c:pt>
-                  <c:pt idx="3">
-                    <c:v>0</c:v>
-                  </c:pt>
-                  <c:pt idx="4">
-                    <c:v>0</c:v>
-                  </c:pt>
-                  <c:pt idx="5">
-                    <c:v>0</c:v>
-                  </c:pt>
-                  <c:pt idx="6">
-                    <c:v>0</c:v>
-                  </c:pt>
-                  <c:pt idx="7">
-                    <c:v>0</c:v>
-                  </c:pt>
-                  <c:pt idx="8">
-                    <c:v>0</c:v>
-                  </c:pt>
-                  <c:pt idx="9">
-                    <c:v>0</c:v>
-                  </c:pt>
-                  <c:pt idx="10">
-                    <c:v>0</c:v>
-                  </c:pt>
-                  <c:pt idx="11">
-                    <c:v>0</c:v>
-                  </c:pt>
-                  <c:pt idx="12">
-                    <c:v>0</c:v>
-                  </c:pt>
-                  <c:pt idx="13">
-                    <c:v>0</c:v>
-                  </c:pt>
-                  <c:pt idx="14">
-                    <c:v>0</c:v>
-                  </c:pt>
-                  <c:pt idx="15">
-                    <c:v>0</c:v>
-                  </c:pt>
-                  <c:pt idx="16">
-                    <c:v>0</c:v>
-                  </c:pt>
-                </c:numCache>
-              </c:numRef>
-            </c:plus>
-            <c:minus>
-              <c:numRef>
-                <c:f>Sheet1!$C$3:$C$19</c:f>
-                <c:numCache>
-                  <c:formatCode>General</c:formatCode>
-                  <c:ptCount val="17"/>
-                  <c:pt idx="0">
-                    <c:v>4.0599999999999996</c:v>
-                  </c:pt>
-                  <c:pt idx="1">
-                    <c:v>0</c:v>
-                  </c:pt>
-                  <c:pt idx="2">
-                    <c:v>0</c:v>
-                  </c:pt>
-                  <c:pt idx="3">
-                    <c:v>0</c:v>
-                  </c:pt>
-                  <c:pt idx="4">
-                    <c:v>0</c:v>
-                  </c:pt>
-                  <c:pt idx="5">
-                    <c:v>0</c:v>
-                  </c:pt>
-                  <c:pt idx="6">
-                    <c:v>0</c:v>
-                  </c:pt>
-                  <c:pt idx="7">
-                    <c:v>0</c:v>
-                  </c:pt>
-                  <c:pt idx="8">
-                    <c:v>0</c:v>
-                  </c:pt>
-                  <c:pt idx="9">
-                    <c:v>0</c:v>
-                  </c:pt>
-                  <c:pt idx="10">
-                    <c:v>0</c:v>
-                  </c:pt>
-                  <c:pt idx="11">
-                    <c:v>0</c:v>
-                  </c:pt>
-                  <c:pt idx="12">
-                    <c:v>0</c:v>
-                  </c:pt>
-                  <c:pt idx="13">
-                    <c:v>0</c:v>
-                  </c:pt>
-                  <c:pt idx="14">
-                    <c:v>0</c:v>
-                  </c:pt>
-                  <c:pt idx="15">
-                    <c:v>0</c:v>
-                  </c:pt>
-                  <c:pt idx="16">
-                    <c:v>0</c:v>
-                  </c:pt>
-                </c:numCache>
-              </c:numRef>
-            </c:minus>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:round/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:errBars>
-          <c:cat>
-            <c:strRef>
-              <c:f>Sheet1!$A$3:$A$19</c:f>
-              <c:strCache>
-                <c:ptCount val="17"/>
-                <c:pt idx="0">
-                  <c:v>GLOBAL Baseline G4400 4GB</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>NA PebbleHost Premium (9900K) 4GB</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>NA EnviroMC Budget (2276G) 4GB</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>EU Birdflop Premium (3900) 4GB</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>NA Birdflop Elite (5950X) 4GB</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>NA DedicatedMC High-End (3900X) 10GB</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>EU DedicatedMC High-End (5950X) 10GB</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>EU EnviroMC Premium (5950X) 10GB</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>EU VolcanoHosting Premium (2643v2) 4GB</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>ASIA Skynode STANDARD-01 (3700X) 2GB</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>EU PebbleHost Premium (9900K) 16GB</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>NA PebbleHost Premium (9900K) 16GB</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>NA PebbleHost Extreme (9900K) 6GB</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>EU PebbleHost Budget (1630v3) 25GB</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>NA PebbleHost Budget (1630v3) 25GB</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>NA Daemex Beta (L5640) 4GB</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>EU PebbleHost Extreme (9900K) 6GB</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$B$3:$B$19</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="17"/>
-                <c:pt idx="0">
-                  <c:v>100</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>49</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>66</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>176</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>211</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>137</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>244</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>164</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>68</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>115</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>67</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>92</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>43</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>87</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>79</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>46</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>78</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-7BBD-4B91-B058-3F82D68DBBC3}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:dLblPos val="outEnd"/>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="1"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:gapWidth val="182"/>
-        <c:axId val="539755408"/>
-        <c:axId val="539752784"/>
-      </c:barChart>
-      <c:catAx>
-        <c:axId val="539755408"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="539752784"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="539752784"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="539755408"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="en-US"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
       <c:tx>
         <c:rich>
           <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
@@ -1118,19 +557,19 @@
                   <c:v>123</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>160</c:v>
+                  <c:v>165</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>160</c:v>
+                  <c:v>182</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>98</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>116</c:v>
+                  <c:v>123</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>126</c:v>
+                  <c:v>124</c:v>
                 </c:pt>
                 <c:pt idx="15">
                   <c:v>82</c:v>
@@ -1309,7 +748,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -1979,46 +1418,6 @@
 </cs:colorStyle>
 </file>
 
-<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
-  <a:schemeClr val="accent1"/>
-  <a:schemeClr val="accent2"/>
-  <a:schemeClr val="accent3"/>
-  <a:schemeClr val="accent4"/>
-  <a:schemeClr val="accent5"/>
-  <a:schemeClr val="accent6"/>
-  <cs:variation/>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-    <a:lumOff val="20000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-    <a:lumOff val="40000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-    <a:lumOff val="30000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-    <a:lumOff val="50000"/>
-  </cs:variation>
-</cs:colorStyle>
-</file>
-
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="216">
   <cs:axisTitle>
@@ -3029,553 +2428,7 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="216">
-  <cs:axisTitle>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:axisTitle>
-  <cs:categoryAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="bg1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:chartArea>
-  <cs:dataLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataLabel>
-  <cs:dataLabelCallout>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
-      <a:spAutoFit/>
-    </cs:bodyPr>
-  </cs:dataLabelCallout>
-  <cs:dataPoint>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint>
-  <cs:dataPoint3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint3D>
-  <cs:dataPointLine>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="28575" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointLine>
-  <cs:dataPointMarker>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
-  <cs:dataPointWireframe>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointWireframe>
-  <cs:dataTable>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataTable>
-  <cs:downBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="75000"/>
-          <a:lumOff val="25000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="50000"/>
-            <a:lumOff val="50000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:seriesLine>
-  <cs:title>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
-  </cs:title>
-  <cs:trendline>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:prstDash val="sysDot"/>
-      </a:ln>
-    </cs:spPr>
-  </cs:trendline>
-  <cs:trendlineLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:trendlineLabel>
-  <cs:upBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:upBar>
-  <cs:valueAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:valueAxis>
-  <cs:wall>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:wall>
-</cs:chartStyle>
-</file>
-
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>395287</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>185737</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>90487</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>71437</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{50FDAAB4-8DD8-42D7-8D05-E4949B834C6E}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -3956,7 +2809,7 @@
   <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B19"/>
+      <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4203,7 +3056,7 @@
         <v>13</v>
       </c>
       <c r="F13">
-        <v>160</v>
+        <v>165</v>
       </c>
       <c r="G13">
         <v>0</v>
@@ -4223,7 +3076,7 @@
         <v>14</v>
       </c>
       <c r="F14">
-        <v>160</v>
+        <v>182</v>
       </c>
       <c r="G14">
         <v>0</v>
@@ -4263,7 +3116,7 @@
         <v>16</v>
       </c>
       <c r="F16">
-        <v>116</v>
+        <v>123</v>
       </c>
       <c r="G16">
         <v>0</v>
@@ -4283,7 +3136,7 @@
         <v>17</v>
       </c>
       <c r="F17">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="G17">
         <v>0</v>
@@ -4319,11 +3172,19 @@
       <c r="C19">
         <v>0</v>
       </c>
+      <c r="E19" t="s">
+        <v>28</v>
+      </c>
+      <c r="F19">
+        <v>95</v>
+      </c>
+      <c r="G19">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
-  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -4332,7 +3193,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S26" sqref="S26"/>
+      <selection activeCell="W20" sqref="W20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
currency conversions API, modify plan naming, add data
</commit_message>
<xml_diff>
--- a/Charts.xlsx
+++ b/Charts.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\akdum\Downloads\GitHub\minecraft-server-hosts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BB82B02-74C6-4443-A4D2-B51B33F5F422}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{796E0034-8433-430D-882E-F6553C4A853C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{44A97144-5CF4-493B-8574-0BA792057902}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{44A97144-5CF4-493B-8574-0BA792057902}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="26">
   <si>
     <t>Plan</t>
   </si>
@@ -67,21 +67,6 @@
     <t>ASIA Skynode STANDARD-01 (3700X) 2GB</t>
   </si>
   <si>
-    <t>EU PebbleHost Premium (9900K) 16GB</t>
-  </si>
-  <si>
-    <t>NA PebbleHost Premium (9900K) 16GB</t>
-  </si>
-  <si>
-    <t>NA PebbleHost Extreme (9900K) 6GB</t>
-  </si>
-  <si>
-    <t>EU PebbleHost Budget (1630v3) 25GB</t>
-  </si>
-  <si>
-    <t>NA PebbleHost Budget (1630v3) 25GB</t>
-  </si>
-  <si>
     <t>NA Daemex Beta (L5640) 4GB</t>
   </si>
   <si>
@@ -112,7 +97,13 @@
     <t>SINGLE</t>
   </si>
   <si>
-    <t>EU PebbleHost Extreme (9900K) 6GB</t>
+    <t>GLOBAL PebbleHost Premium (9900K) 16GB</t>
+  </si>
+  <si>
+    <t>GLOBAL PebbleHost Extreme (9900K) 6GB</t>
+  </si>
+  <si>
+    <t>GLOBAL PebbleHost Budget (1630v3) 25GB</t>
   </si>
 </sst>
 </file>
@@ -168,6 +159,1224 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Single-Thread</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Performance</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="bar"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$B$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Score</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1">
+                <a:lumMod val="40000"/>
+                <a:lumOff val="60000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:errBars>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>Sheet1!$C$3:$C$16</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="14"/>
+                  <c:pt idx="0">
+                    <c:v>4.0599999999999996</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>0</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>0</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>0</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>0</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>0</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>0</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>0</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>0</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>0</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>28.78</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
+                    <c:v>0</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>36.159999999999997</c:v>
+                  </c:pt>
+                  <c:pt idx="13">
+                    <c:v>0</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>Sheet1!$C$3:$C$16</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="14"/>
+                  <c:pt idx="0">
+                    <c:v>4.0599999999999996</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>0</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>0</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>0</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>0</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>0</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>0</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>0</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>0</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>0</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>28.78</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
+                    <c:v>0</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>36.159999999999997</c:v>
+                  </c:pt>
+                  <c:pt idx="13">
+                    <c:v>0</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:alpha val="40000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$3:$A$16</c:f>
+              <c:strCache>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>GLOBAL Baseline G4400 4GB</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>NA PebbleHost Premium (9900K) 4GB</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>NA EnviroMC Budget (2276G) 4GB</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>EU Birdflop Premium (3900) 4GB</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>NA Birdflop Elite (5950X) 4GB</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>NA DedicatedMC High-End (3900X) 10GB</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>EU DedicatedMC High-End (5950X) 10GB</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>EU EnviroMC Premium (5950X) 10GB</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>EU VolcanoHosting Premium (2643v2) 4GB</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>ASIA Skynode STANDARD-01 (3700X) 2GB</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>GLOBAL PebbleHost Premium (9900K) 16GB</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>GLOBAL PebbleHost Extreme (9900K) 6GB</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>GLOBAL PebbleHost Budget (1630v3) 25GB</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>NA Daemex Beta (L5640) 4GB</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$3:$B$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>49</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>66</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>176</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>211</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>137</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>244</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>164</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>68</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>115</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>76</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>63</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>88</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>46</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-F8A6-4B8A-94B4-A8A92DE3BF4A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="outEnd"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="182"/>
+        <c:axId val="477253784"/>
+        <c:axId val="477254112"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="477253784"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="477254112"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="477254112"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Score (Error bars show 95% CI)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="477253784"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Multi-Threaded Performance</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="bar"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$F$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Score</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1">
+                <a:lumMod val="40000"/>
+                <a:lumOff val="60000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:errBars>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>Sheet1!$G$3:$G$16</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="14"/>
+                  <c:pt idx="0">
+                    <c:v>3.27</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>0</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>0</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>0</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>0</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>0</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>0</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>0</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>0</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>0</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>34.049999999999997</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
+                    <c:v>0</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>10.75</c:v>
+                  </c:pt>
+                  <c:pt idx="13">
+                    <c:v>0</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>Sheet1!$G$3:$G$16</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="14"/>
+                  <c:pt idx="0">
+                    <c:v>3.27</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>0</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>0</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>0</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>0</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>0</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>0</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>0</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>0</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>0</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>34.049999999999997</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
+                    <c:v>0</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>10.75</c:v>
+                  </c:pt>
+                  <c:pt idx="13">
+                    <c:v>0</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:alpha val="40000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$E$3:$E$16</c:f>
+              <c:strCache>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>GLOBAL Baseline G4400 4GB</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>US PebbleHost Premium (9900K) 4GB</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>US EnviroMC Budget (2276G) 4GB</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>EU Birdflop Premium (3900) 4GB</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>US Birdflop Premium (3900XT) 4GB</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>US Birdflop Elite (5950X) 4GB</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>US PebbleHost Budget (1630v3) 3GB</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>US DedicatedMC High-End (3900X) 10GB</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>EU DedicatedMC High-End (5950X) 10GB</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>EU Volcano Hosting Premium (2643v2) 4GB</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>GLOBAL PebbleHost Premium (9900K) 16GB</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>GLOBAL PebbleHost Extreme (9900K) 6GB</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>GLOBAL PebbleHost Budget (1630v3) 25GB</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>NA Daemex Beta (L5640) 4GB</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$F$3:$F$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>102</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>197</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>196</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>266</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>58</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>165</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>197</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>123</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>174</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>96</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>124</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>82</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-7E22-43D9-AD12-C2F2238840E1}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="outEnd"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="182"/>
+        <c:axId val="524371024"/>
+        <c:axId val="524369056"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="524371024"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="524369056"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="524369056"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Score (Error bars show 95% CI)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="524371024"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -373,21 +1582,15 @@
                     <c:v>0</c:v>
                   </c:pt>
                   <c:pt idx="10">
-                    <c:v>0</c:v>
+                    <c:v>34.049999999999997</c:v>
                   </c:pt>
                   <c:pt idx="11">
                     <c:v>0</c:v>
                   </c:pt>
                   <c:pt idx="12">
-                    <c:v>0</c:v>
+                    <c:v>10.75</c:v>
                   </c:pt>
                   <c:pt idx="13">
-                    <c:v>0</c:v>
-                  </c:pt>
-                  <c:pt idx="14">
-                    <c:v>0</c:v>
-                  </c:pt>
-                  <c:pt idx="15">
                     <c:v>0</c:v>
                   </c:pt>
                 </c:numCache>
@@ -430,21 +1633,15 @@
                     <c:v>0</c:v>
                   </c:pt>
                   <c:pt idx="10">
-                    <c:v>0</c:v>
+                    <c:v>34.049999999999997</c:v>
                   </c:pt>
                   <c:pt idx="11">
                     <c:v>0</c:v>
                   </c:pt>
                   <c:pt idx="12">
-                    <c:v>0</c:v>
+                    <c:v>10.75</c:v>
                   </c:pt>
                   <c:pt idx="13">
-                    <c:v>0</c:v>
-                  </c:pt>
-                  <c:pt idx="14">
-                    <c:v>0</c:v>
-                  </c:pt>
-                  <c:pt idx="15">
                     <c:v>0</c:v>
                   </c:pt>
                 </c:numCache>
@@ -468,7 +1665,7 @@
             <c:strRef>
               <c:f>Sheet1!$E$3:$E$18</c:f>
               <c:strCache>
-                <c:ptCount val="16"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
                   <c:v>GLOBAL Baseline G4400 4GB</c:v>
                 </c:pt>
@@ -500,21 +1697,15 @@
                   <c:v>EU Volcano Hosting Premium (2643v2) 4GB</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>EU PebbleHost Premium (9900K) 16GB</c:v>
+                  <c:v>GLOBAL PebbleHost Premium (9900K) 16GB</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>NA PebbleHost Premium (9900K) 16GB</c:v>
+                  <c:v>GLOBAL PebbleHost Extreme (9900K) 6GB</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>NA PebbleHost Extreme (9900K) 6GB</c:v>
+                  <c:v>GLOBAL PebbleHost Budget (1630v3) 25GB</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>EU PebbleHost Budget (1630v3) 25GB</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>NA PebbleHost Budget (1630v3) 25GB</c:v>
-                </c:pt>
-                <c:pt idx="15">
                   <c:v>NA Daemex Beta (L5640) 4GB</c:v>
                 </c:pt>
               </c:strCache>
@@ -557,21 +1748,15 @@
                   <c:v>123</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>165</c:v>
+                  <c:v>174</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>182</c:v>
+                  <c:v>96</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>98</c:v>
+                  <c:v>124</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>123</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>124</c:v>
-                </c:pt>
-                <c:pt idx="15">
                   <c:v>82</c:v>
                 </c:pt>
               </c:numCache>
@@ -748,7 +1933,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -951,24 +2136,15 @@
                     <c:v>0</c:v>
                   </c:pt>
                   <c:pt idx="10">
-                    <c:v>0</c:v>
+                    <c:v>28.78</c:v>
                   </c:pt>
                   <c:pt idx="11">
                     <c:v>0</c:v>
                   </c:pt>
                   <c:pt idx="12">
-                    <c:v>0</c:v>
+                    <c:v>36.159999999999997</c:v>
                   </c:pt>
                   <c:pt idx="13">
-                    <c:v>0</c:v>
-                  </c:pt>
-                  <c:pt idx="14">
-                    <c:v>0</c:v>
-                  </c:pt>
-                  <c:pt idx="15">
-                    <c:v>0</c:v>
-                  </c:pt>
-                  <c:pt idx="16">
                     <c:v>0</c:v>
                   </c:pt>
                 </c:numCache>
@@ -1011,24 +2187,15 @@
                     <c:v>0</c:v>
                   </c:pt>
                   <c:pt idx="10">
-                    <c:v>0</c:v>
+                    <c:v>28.78</c:v>
                   </c:pt>
                   <c:pt idx="11">
                     <c:v>0</c:v>
                   </c:pt>
                   <c:pt idx="12">
-                    <c:v>0</c:v>
+                    <c:v>36.159999999999997</c:v>
                   </c:pt>
                   <c:pt idx="13">
-                    <c:v>0</c:v>
-                  </c:pt>
-                  <c:pt idx="14">
-                    <c:v>0</c:v>
-                  </c:pt>
-                  <c:pt idx="15">
-                    <c:v>0</c:v>
-                  </c:pt>
-                  <c:pt idx="16">
                     <c:v>0</c:v>
                   </c:pt>
                 </c:numCache>
@@ -1052,7 +2219,7 @@
             <c:strRef>
               <c:f>Sheet1!$A$3:$A$19</c:f>
               <c:strCache>
-                <c:ptCount val="17"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
                   <c:v>GLOBAL Baseline G4400 4GB</c:v>
                 </c:pt>
@@ -1084,25 +2251,16 @@
                   <c:v>ASIA Skynode STANDARD-01 (3700X) 2GB</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>EU PebbleHost Premium (9900K) 16GB</c:v>
+                  <c:v>GLOBAL PebbleHost Premium (9900K) 16GB</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>NA PebbleHost Premium (9900K) 16GB</c:v>
+                  <c:v>GLOBAL PebbleHost Extreme (9900K) 6GB</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>NA PebbleHost Extreme (9900K) 6GB</c:v>
+                  <c:v>GLOBAL PebbleHost Budget (1630v3) 25GB</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>EU PebbleHost Budget (1630v3) 25GB</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>NA PebbleHost Budget (1630v3) 25GB</c:v>
-                </c:pt>
-                <c:pt idx="15">
                   <c:v>NA Daemex Beta (L5640) 4GB</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>EU PebbleHost Extreme (9900K) 6GB</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1144,25 +2302,16 @@
                   <c:v>115</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>67</c:v>
+                  <c:v>76</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>92</c:v>
+                  <c:v>63</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>43</c:v>
+                  <c:v>88</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>87</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>79</c:v>
-                </c:pt>
-                <c:pt idx="15">
                   <c:v>46</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>78</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1418,6 +2567,86 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="216">
   <cs:axisTitle>
@@ -2428,18 +3657,1105 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="216">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="216">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>600075</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{27FAE170-8303-4E95-B987-FCD6667FA0DE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>185737</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>600075</xdr:colOff>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{422E965A-A010-439A-AEC2-0920F889BCFD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>23</xdr:col>
-      <xdr:colOff>23813</xdr:colOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>600075</xdr:colOff>
       <xdr:row>16</xdr:row>
       <xdr:rowOff>100013</xdr:rowOff>
     </xdr:to>
@@ -2476,8 +4792,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
       <xdr:row>16</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
@@ -2806,20 +5122,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{049E8E79-07BD-45DF-9A6A-257E2C4C3481}">
-  <dimension ref="A1:G19"/>
+  <dimension ref="A1:G16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="R37" sqref="R37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="E1" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -2873,7 +5189,7 @@
         <v>0</v>
       </c>
       <c r="E4" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="F4">
         <v>45</v>
@@ -2893,7 +5209,7 @@
         <v>0</v>
       </c>
       <c r="E5" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="F5">
         <v>102</v>
@@ -2933,7 +5249,7 @@
         <v>0</v>
       </c>
       <c r="E7" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="F7">
         <v>196</v>
@@ -2953,7 +5269,7 @@
         <v>0</v>
       </c>
       <c r="E8" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="F8">
         <v>266</v>
@@ -2973,7 +5289,7 @@
         <v>0</v>
       </c>
       <c r="E9" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="F9">
         <v>58</v>
@@ -2993,7 +5309,7 @@
         <v>0</v>
       </c>
       <c r="E10" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="F10">
         <v>165</v>
@@ -3033,7 +5349,7 @@
         <v>0</v>
       </c>
       <c r="E12" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="F12">
         <v>123</v>
@@ -3044,39 +5360,39 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="B13">
-        <v>67</v>
+        <v>76</v>
       </c>
       <c r="C13">
-        <v>0</v>
+        <v>28.78</v>
       </c>
       <c r="E13" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="F13">
-        <v>165</v>
+        <v>174</v>
       </c>
       <c r="G13">
-        <v>0</v>
+        <v>34.049999999999997</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="B14">
-        <v>92</v>
+        <v>63</v>
       </c>
       <c r="C14">
         <v>0</v>
       </c>
       <c r="E14" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="F14">
-        <v>182</v>
+        <v>96</v>
       </c>
       <c r="G14">
         <v>0</v>
@@ -3084,107 +5400,48 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="B15">
-        <v>43</v>
+        <v>88</v>
       </c>
       <c r="C15">
-        <v>0</v>
+        <v>36.159999999999997</v>
       </c>
       <c r="E15" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="F15">
-        <v>98</v>
+        <v>124</v>
       </c>
       <c r="G15">
-        <v>0</v>
+        <v>10.75</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B16">
-        <v>87</v>
+        <v>46</v>
       </c>
       <c r="C16">
         <v>0</v>
       </c>
       <c r="E16" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="F16">
-        <v>123</v>
+        <v>82</v>
       </c>
       <c r="G16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>17</v>
-      </c>
-      <c r="B17">
-        <v>79</v>
-      </c>
-      <c r="C17">
-        <v>0</v>
-      </c>
-      <c r="E17" t="s">
-        <v>17</v>
-      </c>
-      <c r="F17">
-        <v>124</v>
-      </c>
-      <c r="G17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>18</v>
-      </c>
-      <c r="B18">
-        <v>46</v>
-      </c>
-      <c r="C18">
-        <v>0</v>
-      </c>
-      <c r="E18" t="s">
-        <v>18</v>
-      </c>
-      <c r="F18">
-        <v>82</v>
-      </c>
-      <c r="G18">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>28</v>
-      </c>
-      <c r="B19">
-        <v>78</v>
-      </c>
-      <c r="C19">
-        <v>0</v>
-      </c>
-      <c r="E19" t="s">
-        <v>28</v>
-      </c>
-      <c r="F19">
-        <v>95</v>
-      </c>
-      <c r="G19">
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -3192,8 +5449,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42532320-4BB7-4186-A5F1-675B70719D59}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="W20" sqref="W20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="X9" sqref="X9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
add data and sort results by price
</commit_message>
<xml_diff>
--- a/Charts.xlsx
+++ b/Charts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\akdum\Downloads\GitHub\minecraft-server-hosts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27DC1A81-D085-4849-AEC9-320EAD9D65A6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6A4CB61-BEDC-4CCA-AD3E-AAB530F0DC87}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{44A97144-5CF4-493B-8574-0BA792057902}"/>
   </bookViews>
@@ -43,9 +43,6 @@
   </si>
   <si>
     <t>GLOBAL Baseline G4400 4GB (N/A)</t>
-  </si>
-  <si>
-    <t>EU Volcano Hosting Premium 4GB ($9.54)</t>
   </si>
   <si>
     <t>NA PebbleHost Premium 4GB ($9.00)</t>
@@ -91,6 +88,9 @@
   </si>
   <si>
     <t>ASIA Skynode STANDARD-01 2GB ($25.00)</t>
+  </si>
+  <si>
+    <t>EU Volcano Hosting Premium 4GB ($9.51)</t>
   </si>
 </sst>
 </file>
@@ -321,46 +321,46 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="14"/>
                   <c:pt idx="0">
+                    <c:v>54.98</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>0</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>0</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>28.78</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>0</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>0</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>36.159999999999997</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>0</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>0</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>0</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>0</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
+                    <c:v>0</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>0</c:v>
+                  </c:pt>
+                  <c:pt idx="13">
                     <c:v>4.0599999999999996</c:v>
-                  </c:pt>
-                  <c:pt idx="1">
-                    <c:v>0</c:v>
-                  </c:pt>
-                  <c:pt idx="2">
-                    <c:v>0</c:v>
-                  </c:pt>
-                  <c:pt idx="3">
-                    <c:v>0</c:v>
-                  </c:pt>
-                  <c:pt idx="4">
-                    <c:v>0</c:v>
-                  </c:pt>
-                  <c:pt idx="5">
-                    <c:v>0</c:v>
-                  </c:pt>
-                  <c:pt idx="6">
-                    <c:v>0</c:v>
-                  </c:pt>
-                  <c:pt idx="7">
-                    <c:v>0</c:v>
-                  </c:pt>
-                  <c:pt idx="8">
-                    <c:v>0</c:v>
-                  </c:pt>
-                  <c:pt idx="9">
-                    <c:v>0</c:v>
-                  </c:pt>
-                  <c:pt idx="10">
-                    <c:v>28.78</c:v>
-                  </c:pt>
-                  <c:pt idx="11">
-                    <c:v>0</c:v>
-                  </c:pt>
-                  <c:pt idx="12">
-                    <c:v>36.159999999999997</c:v>
-                  </c:pt>
-                  <c:pt idx="13">
-                    <c:v>0</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -372,46 +372,46 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="14"/>
                   <c:pt idx="0">
+                    <c:v>54.98</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>0</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>0</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>28.78</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>0</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>0</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>36.159999999999997</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>0</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>0</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>0</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>0</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
+                    <c:v>0</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>0</c:v>
+                  </c:pt>
+                  <c:pt idx="13">
                     <c:v>4.0599999999999996</c:v>
-                  </c:pt>
-                  <c:pt idx="1">
-                    <c:v>0</c:v>
-                  </c:pt>
-                  <c:pt idx="2">
-                    <c:v>0</c:v>
-                  </c:pt>
-                  <c:pt idx="3">
-                    <c:v>0</c:v>
-                  </c:pt>
-                  <c:pt idx="4">
-                    <c:v>0</c:v>
-                  </c:pt>
-                  <c:pt idx="5">
-                    <c:v>0</c:v>
-                  </c:pt>
-                  <c:pt idx="6">
-                    <c:v>0</c:v>
-                  </c:pt>
-                  <c:pt idx="7">
-                    <c:v>0</c:v>
-                  </c:pt>
-                  <c:pt idx="8">
-                    <c:v>0</c:v>
-                  </c:pt>
-                  <c:pt idx="9">
-                    <c:v>0</c:v>
-                  </c:pt>
-                  <c:pt idx="10">
-                    <c:v>28.78</c:v>
-                  </c:pt>
-                  <c:pt idx="11">
-                    <c:v>0</c:v>
-                  </c:pt>
-                  <c:pt idx="12">
-                    <c:v>36.159999999999997</c:v>
-                  </c:pt>
-                  <c:pt idx="13">
-                    <c:v>0</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -435,46 +435,46 @@
               <c:strCache>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
+                  <c:v>GLOBAL PebbleHost Extreme 6GB ($37.50)</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>NA DedicatedMC High-End 10GB ($36.00)</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>EU DedicatedMC High-End 10GB ($36.00)</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>GLOBAL PebbleHost Premium 16GB ($36.00)</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>EU EnviroMC Premium 10GB ($25.00)</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>ASIA Skynode STANDARD-01 2GB ($25.00)</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>GLOBAL PebbleHost Budget 25GB ($25.00)</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>NA Birdflop Elite 4GB ($12.00)</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>NA PebbleHost Premium 4GB ($9.00)</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>EU Birdflop Premium 4GB ($8.00)</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>EU VolcanoHosting Premium 4GB ($8.00)</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>NA EnviroMC Budget 4GB ($4.00)</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>NA Daemex Beta 4GB ($0.00)</c:v>
+                </c:pt>
+                <c:pt idx="13">
                   <c:v>GLOBAL Baseline G4400 4GB (N/A)</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>NA PebbleHost Premium 4GB ($9.00)</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>NA EnviroMC Budget 4GB ($4.00)</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>EU Birdflop Premium 4GB ($8.00)</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>NA Birdflop Elite 4GB ($12.00)</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>NA DedicatedMC High-End 10GB ($36.00)</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>EU DedicatedMC High-End 10GB ($36.00)</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>EU EnviroMC Premium 10GB ($25.00)</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>EU VolcanoHosting Premium 4GB ($8.00)</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>ASIA Skynode STANDARD-01 2GB ($25.00)</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>GLOBAL PebbleHost Premium 16GB ($36.00)</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>GLOBAL PebbleHost Extreme 6GB ($37.50)</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>GLOBAL PebbleHost Budget 25GB ($25.00)</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>NA Daemex Beta 4GB ($0.00)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -486,46 +486,46 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
+                  <c:v>68</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>137</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>244</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>76</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>164</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>115</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>88</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>211</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>49</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>176</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>68</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>66</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>46</c:v>
+                </c:pt>
+                <c:pt idx="13">
                   <c:v>100</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>49</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>66</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>176</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>211</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>137</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>244</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>164</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>68</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>115</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>76</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>63</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>88</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>46</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -928,46 +928,46 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="14"/>
                   <c:pt idx="0">
+                    <c:v>0</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>0</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>0</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>34.049999999999997</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>10.75</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>0</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>0</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>0</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>0</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>0</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>0</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
+                    <c:v>0</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>0</c:v>
+                  </c:pt>
+                  <c:pt idx="13">
                     <c:v>3.27</c:v>
-                  </c:pt>
-                  <c:pt idx="1">
-                    <c:v>0</c:v>
-                  </c:pt>
-                  <c:pt idx="2">
-                    <c:v>0</c:v>
-                  </c:pt>
-                  <c:pt idx="3">
-                    <c:v>0</c:v>
-                  </c:pt>
-                  <c:pt idx="4">
-                    <c:v>0</c:v>
-                  </c:pt>
-                  <c:pt idx="5">
-                    <c:v>0</c:v>
-                  </c:pt>
-                  <c:pt idx="6">
-                    <c:v>0</c:v>
-                  </c:pt>
-                  <c:pt idx="7">
-                    <c:v>0</c:v>
-                  </c:pt>
-                  <c:pt idx="8">
-                    <c:v>0</c:v>
-                  </c:pt>
-                  <c:pt idx="9">
-                    <c:v>0</c:v>
-                  </c:pt>
-                  <c:pt idx="10">
-                    <c:v>34.049999999999997</c:v>
-                  </c:pt>
-                  <c:pt idx="11">
-                    <c:v>0</c:v>
-                  </c:pt>
-                  <c:pt idx="12">
-                    <c:v>10.75</c:v>
-                  </c:pt>
-                  <c:pt idx="13">
-                    <c:v>0</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -979,46 +979,46 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="14"/>
                   <c:pt idx="0">
+                    <c:v>0</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>0</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>0</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>34.049999999999997</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>10.75</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>0</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>0</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>0</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>0</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>0</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>0</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
+                    <c:v>0</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>0</c:v>
+                  </c:pt>
+                  <c:pt idx="13">
                     <c:v>3.27</c:v>
-                  </c:pt>
-                  <c:pt idx="1">
-                    <c:v>0</c:v>
-                  </c:pt>
-                  <c:pt idx="2">
-                    <c:v>0</c:v>
-                  </c:pt>
-                  <c:pt idx="3">
-                    <c:v>0</c:v>
-                  </c:pt>
-                  <c:pt idx="4">
-                    <c:v>0</c:v>
-                  </c:pt>
-                  <c:pt idx="5">
-                    <c:v>0</c:v>
-                  </c:pt>
-                  <c:pt idx="6">
-                    <c:v>0</c:v>
-                  </c:pt>
-                  <c:pt idx="7">
-                    <c:v>0</c:v>
-                  </c:pt>
-                  <c:pt idx="8">
-                    <c:v>0</c:v>
-                  </c:pt>
-                  <c:pt idx="9">
-                    <c:v>0</c:v>
-                  </c:pt>
-                  <c:pt idx="10">
-                    <c:v>34.049999999999997</c:v>
-                  </c:pt>
-                  <c:pt idx="11">
-                    <c:v>0</c:v>
-                  </c:pt>
-                  <c:pt idx="12">
-                    <c:v>10.75</c:v>
-                  </c:pt>
-                  <c:pt idx="13">
-                    <c:v>0</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -1042,46 +1042,46 @@
               <c:strCache>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
+                  <c:v>GLOBAL PebbleHost Extreme 6GB ($37.50)</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>NA DedicatedMC High-End 10GB ($36.00)</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>EU DedicatedMC High-End 10GB ($36.00)</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>GLOBAL PebbleHost Premium 16GB ($36.00)</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>GLOBAL PebbleHost Budget 25GB ($25.00)</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>NA Birdflop Premium 4GB ($12.00)</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>NA Birdflop Elite 4GB ($12.00)</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>EU Volcano Hosting Premium 4GB ($9.51)</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>NA PebbleHost Premium 4GB ($9.00)</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>EU Birdflop Premium 4GB ($8.00)</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>NA EnviroMC Budget 4GB ($4.00)</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>NA PebbleHost Budget 3GB ($3.00)</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>NA Daemex Beta 4GB ($0.00)</c:v>
+                </c:pt>
+                <c:pt idx="13">
                   <c:v>GLOBAL Baseline G4400 4GB (N/A)</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>NA PebbleHost Premium 4GB ($9.00)</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>NA EnviroMC Budget 4GB ($4.00)</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>EU Birdflop Premium 4GB ($8.00)</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>NA Birdflop Premium 4GB ($12.00)</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>NA Birdflop Elite 4GB ($12.00)</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>NA PebbleHost Budget 3GB ($3.00)</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>NA DedicatedMC High-End 10GB ($36.00)</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>EU DedicatedMC High-End 10GB ($36.00)</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>EU Volcano Hosting Premium 4GB ($9.54)</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>GLOBAL PebbleHost Premium 16GB ($36.00)</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>GLOBAL PebbleHost Extreme 6GB ($37.50)</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>GLOBAL PebbleHost Budget 25GB ($25.00)</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>NA Daemex Beta 4GB ($0.00)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1093,46 +1093,46 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
+                  <c:v>96</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>165</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>197</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>174</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>124</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>196</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>266</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>123</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>197</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>102</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>58</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>82</c:v>
+                </c:pt>
+                <c:pt idx="13">
                   <c:v>100</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>45</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>102</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>197</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>196</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>266</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>58</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>165</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>197</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>123</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>174</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>96</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>124</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>82</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2830,7 +2830,7 @@
   <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="P33" sqref="P33"/>
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2865,39 +2865,39 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="B3">
-        <v>100</v>
+        <v>68</v>
       </c>
       <c r="C3">
-        <v>4.0599999999999996</v>
+        <v>54.98</v>
       </c>
       <c r="E3" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="F3">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="G3">
-        <v>3.27</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="B4">
-        <v>49</v>
+        <v>137</v>
       </c>
       <c r="C4">
         <v>0</v>
       </c>
       <c r="E4" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="F4">
-        <v>45</v>
+        <v>165</v>
       </c>
       <c r="G4">
         <v>0</v>
@@ -2905,19 +2905,19 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="B5">
-        <v>66</v>
+        <v>244</v>
       </c>
       <c r="C5">
         <v>0</v>
       </c>
       <c r="E5" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="F5">
-        <v>102</v>
+        <v>197</v>
       </c>
       <c r="G5">
         <v>0</v>
@@ -2925,59 +2925,59 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="B6">
-        <v>176</v>
+        <v>76</v>
       </c>
       <c r="C6">
-        <v>0</v>
+        <v>28.78</v>
       </c>
       <c r="E6" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="F6">
-        <v>197</v>
+        <v>174</v>
       </c>
       <c r="G6">
-        <v>0</v>
+        <v>34.049999999999997</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="B7">
-        <v>211</v>
+        <v>164</v>
       </c>
       <c r="C7">
         <v>0</v>
       </c>
       <c r="E7" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="F7">
-        <v>196</v>
+        <v>124</v>
       </c>
       <c r="G7">
-        <v>0</v>
+        <v>10.75</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="B8">
-        <v>137</v>
+        <v>115</v>
       </c>
       <c r="C8">
         <v>0</v>
       </c>
       <c r="E8" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F8">
-        <v>266</v>
+        <v>196</v>
       </c>
       <c r="G8">
         <v>0</v>
@@ -2985,19 +2985,19 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B9">
-        <v>244</v>
+        <v>88</v>
       </c>
       <c r="C9">
-        <v>0</v>
+        <v>36.159999999999997</v>
       </c>
       <c r="E9" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F9">
-        <v>58</v>
+        <v>266</v>
       </c>
       <c r="G9">
         <v>0</v>
@@ -3005,19 +3005,19 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="B10">
-        <v>164</v>
+        <v>211</v>
       </c>
       <c r="C10">
         <v>0</v>
       </c>
       <c r="E10" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="F10">
-        <v>165</v>
+        <v>123</v>
       </c>
       <c r="G10">
         <v>0</v>
@@ -3025,19 +3025,19 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="B11">
-        <v>68</v>
+        <v>49</v>
       </c>
       <c r="C11">
         <v>0</v>
       </c>
       <c r="E11" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="F11">
-        <v>197</v>
+        <v>45</v>
       </c>
       <c r="G11">
         <v>0</v>
@@ -3045,19 +3045,19 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="B12">
-        <v>115</v>
+        <v>176</v>
       </c>
       <c r="C12">
         <v>0</v>
       </c>
       <c r="E12" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="F12">
-        <v>123</v>
+        <v>197</v>
       </c>
       <c r="G12">
         <v>0</v>
@@ -3065,39 +3065,39 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="B13">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="C13">
-        <v>28.78</v>
+        <v>0</v>
       </c>
       <c r="E13" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="F13">
-        <v>174</v>
+        <v>102</v>
       </c>
       <c r="G13">
-        <v>34.049999999999997</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="B14">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="C14">
         <v>0</v>
       </c>
       <c r="E14" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="F14">
-        <v>96</v>
+        <v>58</v>
       </c>
       <c r="G14">
         <v>0</v>
@@ -3108,39 +3108,39 @@
         <v>17</v>
       </c>
       <c r="B15">
-        <v>88</v>
+        <v>46</v>
       </c>
       <c r="C15">
-        <v>36.159999999999997</v>
+        <v>0</v>
       </c>
       <c r="E15" t="s">
         <v>17</v>
       </c>
       <c r="F15">
-        <v>124</v>
+        <v>82</v>
       </c>
       <c r="G15">
-        <v>10.75</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>18</v>
+        <v>5</v>
       </c>
       <c r="B16">
-        <v>46</v>
+        <v>100</v>
       </c>
       <c r="C16">
-        <v>0</v>
+        <v>4.0599999999999996</v>
       </c>
       <c r="E16" t="s">
-        <v>18</v>
+        <v>5</v>
       </c>
       <c r="F16">
-        <v>82</v>
+        <v>100</v>
       </c>
       <c r="G16">
-        <v>0</v>
+        <v>3.27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix currency conversions for single-thread and add data
</commit_message>
<xml_diff>
--- a/Charts.xlsx
+++ b/Charts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\akdum\Downloads\GitHub\minecraft-server-hosts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6A4CB61-BEDC-4CCA-AD3E-AAB530F0DC87}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39959617-787B-48E6-82CF-90AF41155D0D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{44A97144-5CF4-493B-8574-0BA792057902}"/>
   </bookViews>
@@ -84,13 +84,13 @@
     <t>EU EnviroMC Premium 10GB ($25.00)</t>
   </si>
   <si>
-    <t>EU VolcanoHosting Premium 4GB ($8.00)</t>
-  </si>
-  <si>
     <t>ASIA Skynode STANDARD-01 2GB ($25.00)</t>
   </si>
   <si>
     <t>EU Volcano Hosting Premium 4GB ($9.51)</t>
+  </si>
+  <si>
+    <t>EU VolcanoHosting Premium 4GB ($9.51)</t>
   </si>
 </sst>
 </file>
@@ -459,13 +459,13 @@
                   <c:v>NA Birdflop Elite 4GB ($12.00)</c:v>
                 </c:pt>
                 <c:pt idx="8">
+                  <c:v>EU VolcanoHosting Premium 4GB ($9.51)</c:v>
+                </c:pt>
+                <c:pt idx="9">
                   <c:v>NA PebbleHost Premium 4GB ($9.00)</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>EU Birdflop Premium 4GB ($8.00)</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>EU VolcanoHosting Premium 4GB ($8.00)</c:v>
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>NA EnviroMC Budget 4GB ($4.00)</c:v>
@@ -510,13 +510,13 @@
                   <c:v>211</c:v>
                 </c:pt>
                 <c:pt idx="8">
+                  <c:v>68</c:v>
+                </c:pt>
+                <c:pt idx="9">
                   <c:v>49</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>176</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>68</c:v>
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>66</c:v>
@@ -928,7 +928,7 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="14"/>
                   <c:pt idx="0">
-                    <c:v>0</c:v>
+                    <c:v>38.43</c:v>
                   </c:pt>
                   <c:pt idx="1">
                     <c:v>0</c:v>
@@ -979,7 +979,7 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="14"/>
                   <c:pt idx="0">
-                    <c:v>0</c:v>
+                    <c:v>38.43</c:v>
                   </c:pt>
                   <c:pt idx="1">
                     <c:v>0</c:v>
@@ -1093,7 +1093,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
-                  <c:v>96</c:v>
+                  <c:v>105</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>165</c:v>
@@ -2830,7 +2830,7 @@
   <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+      <selection activeCell="V20" sqref="V20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2877,10 +2877,10 @@
         <v>15</v>
       </c>
       <c r="F3">
-        <v>96</v>
+        <v>105</v>
       </c>
       <c r="G3">
-        <v>0</v>
+        <v>38.43</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -2965,7 +2965,7 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B8">
         <v>115</v>
@@ -3014,7 +3014,7 @@
         <v>0</v>
       </c>
       <c r="E10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F10">
         <v>123</v>
@@ -3025,10 +3025,10 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>6</v>
+        <v>21</v>
       </c>
       <c r="B11">
-        <v>49</v>
+        <v>68</v>
       </c>
       <c r="C11">
         <v>0</v>
@@ -3045,10 +3045,10 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B12">
-        <v>176</v>
+        <v>49</v>
       </c>
       <c r="C12">
         <v>0</v>
@@ -3065,10 +3065,10 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="B13">
-        <v>68</v>
+        <v>176</v>
       </c>
       <c r="C13">
         <v>0</v>

</xml_diff>

<commit_message>
Add data & rename tests
</commit_message>
<xml_diff>
--- a/Charts.xlsx
+++ b/Charts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\akdum\Downloads\GitHub\minecraft-server-hosts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8726926C-F0ED-4536-8D38-568F649465A3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80D8C59C-F79C-4A31-AFF7-44F4E9FB16F3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{44A97144-5CF4-493B-8574-0BA792057902}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="24">
   <si>
     <t>Plan</t>
   </si>
@@ -81,16 +81,22 @@
     <t>EU EnviroMC Premium 10GB ($25.00)</t>
   </si>
   <si>
-    <t>EU Volcano Hosting Premium 4GB ($9.51)</t>
-  </si>
-  <si>
-    <t>EU VolcanoHosting Premium 4GB ($9.51)</t>
-  </si>
-  <si>
     <t>NA Birdflop Elite 8GB ($24.00)</t>
   </si>
   <si>
     <t>ASIA Skynode STANDARD-01 2GB ($5.00)</t>
+  </si>
+  <si>
+    <t>EU BloomHost Performance+ 8GB ($22.00)</t>
+  </si>
+  <si>
+    <t>EU BloomHost Performance 8GB ($16.00)</t>
+  </si>
+  <si>
+    <t>EU VolcanoHosting Premium 4GB ($9.43)</t>
+  </si>
+  <si>
+    <t>EU Volcano Hosting Premium 4GB ($9.43)</t>
   </si>
 </sst>
 </file>
@@ -180,11 +186,11 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Single-Thread</a:t>
+              <a:t>Entity Tick</a:t>
             </a:r>
             <a:r>
               <a:rPr lang="en-US" baseline="0"/>
-              <a:t> Performance</a:t>
+              <a:t> Score</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -316,10 +322,10 @@
             <c:noEndCap val="0"/>
             <c:plus>
               <c:numRef>
-                <c:f>Sheet1!$C$3:$C$16</c:f>
+                <c:f>Sheet1!$C$3:$C$18</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
-                  <c:ptCount val="14"/>
+                  <c:ptCount val="16"/>
                   <c:pt idx="0">
                     <c:v>54.98</c:v>
                   </c:pt>
@@ -360,6 +366,12 @@
                     <c:v>0</c:v>
                   </c:pt>
                   <c:pt idx="13">
+                    <c:v>0</c:v>
+                  </c:pt>
+                  <c:pt idx="14">
+                    <c:v>0</c:v>
+                  </c:pt>
+                  <c:pt idx="15">
                     <c:v>4.0599999999999996</c:v>
                   </c:pt>
                 </c:numCache>
@@ -367,10 +379,10 @@
             </c:plus>
             <c:minus>
               <c:numRef>
-                <c:f>Sheet1!$C$3:$C$16</c:f>
+                <c:f>Sheet1!$C$3:$C$18</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
-                  <c:ptCount val="14"/>
+                  <c:ptCount val="16"/>
                   <c:pt idx="0">
                     <c:v>54.98</c:v>
                   </c:pt>
@@ -411,6 +423,12 @@
                     <c:v>0</c:v>
                   </c:pt>
                   <c:pt idx="13">
+                    <c:v>0</c:v>
+                  </c:pt>
+                  <c:pt idx="14">
+                    <c:v>0</c:v>
+                  </c:pt>
+                  <c:pt idx="15">
                     <c:v>4.0599999999999996</c:v>
                   </c:pt>
                 </c:numCache>
@@ -431,9 +449,9 @@
           </c:errBars>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$3:$A$16</c:f>
+              <c:f>Sheet1!$A$3:$A$18</c:f>
               <c:strCache>
-                <c:ptCount val="14"/>
+                <c:ptCount val="16"/>
                 <c:pt idx="0">
                   <c:v>GLOBAL PebbleHost Extreme 6GB ($37.50)</c:v>
                 </c:pt>
@@ -456,24 +474,30 @@
                   <c:v>NA Birdflop Elite 8GB ($24.00)</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>EU VolcanoHosting Premium 4GB ($9.51)</c:v>
+                  <c:v>EU BloomHost Performance+ 8GB ($22.00)</c:v>
                 </c:pt>
                 <c:pt idx="8">
+                  <c:v>EU BloomHost Performance 8GB ($16.00)</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>EU VolcanoHosting Premium 4GB ($9.43)</c:v>
+                </c:pt>
+                <c:pt idx="10">
                   <c:v>NA PebbleHost Premium 4GB ($9.00)</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="11">
                   <c:v>EU Birdflop Premium 4GB ($8.00)</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="12">
                   <c:v>ASIA Skynode STANDARD-01 2GB ($5.00)</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="13">
                   <c:v>NA EnviroMC Budget 4GB ($4.00)</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="14">
                   <c:v>NA Daemex Beta 4GB ($0.00)</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="15">
                   <c:v>GLOBAL Baseline G4400 4GB (N/A)</c:v>
                 </c:pt>
               </c:strCache>
@@ -481,10 +505,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$3:$B$16</c:f>
+              <c:f>Sheet1!$B$3:$B$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="14"/>
+                <c:ptCount val="16"/>
                 <c:pt idx="0">
                   <c:v>68</c:v>
                 </c:pt>
@@ -507,24 +531,30 @@
                   <c:v>196</c:v>
                 </c:pt>
                 <c:pt idx="7">
+                  <c:v>210</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>137</c:v>
+                </c:pt>
+                <c:pt idx="9">
                   <c:v>68</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="10">
                   <c:v>49</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="11">
                   <c:v>176</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="12">
                   <c:v>115</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="13">
                   <c:v>66</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="14">
                   <c:v>46</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="15">
                   <c:v>100</c:v>
                 </c:pt>
               </c:numCache>
@@ -791,7 +821,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Multi-Threaded Performance</a:t>
+              <a:t>Chunk Generation Score</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -923,10 +953,10 @@
             <c:noEndCap val="0"/>
             <c:plus>
               <c:numRef>
-                <c:f>Sheet1!$G$3:$G$16</c:f>
+                <c:f>Sheet1!$G$3:$G$18</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
-                  <c:ptCount val="14"/>
+                  <c:ptCount val="16"/>
                   <c:pt idx="0">
                     <c:v>38.43</c:v>
                   </c:pt>
@@ -967,6 +997,12 @@
                     <c:v>0</c:v>
                   </c:pt>
                   <c:pt idx="13">
+                    <c:v>0</c:v>
+                  </c:pt>
+                  <c:pt idx="14">
+                    <c:v>0</c:v>
+                  </c:pt>
+                  <c:pt idx="15">
                     <c:v>3.27</c:v>
                   </c:pt>
                 </c:numCache>
@@ -974,10 +1010,10 @@
             </c:plus>
             <c:minus>
               <c:numRef>
-                <c:f>Sheet1!$G$3:$G$16</c:f>
+                <c:f>Sheet1!$G$3:$G$18</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
-                  <c:ptCount val="14"/>
+                  <c:ptCount val="16"/>
                   <c:pt idx="0">
                     <c:v>38.43</c:v>
                   </c:pt>
@@ -1018,6 +1054,12 @@
                     <c:v>0</c:v>
                   </c:pt>
                   <c:pt idx="13">
+                    <c:v>0</c:v>
+                  </c:pt>
+                  <c:pt idx="14">
+                    <c:v>0</c:v>
+                  </c:pt>
+                  <c:pt idx="15">
                     <c:v>3.27</c:v>
                   </c:pt>
                 </c:numCache>
@@ -1038,9 +1080,9 @@
           </c:errBars>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$E$3:$E$16</c:f>
+              <c:f>Sheet1!$E$3:$E$18</c:f>
               <c:strCache>
-                <c:ptCount val="14"/>
+                <c:ptCount val="16"/>
                 <c:pt idx="0">
                   <c:v>GLOBAL PebbleHost Extreme 6GB ($37.50)</c:v>
                 </c:pt>
@@ -1060,27 +1102,33 @@
                   <c:v>NA Birdflop Elite 8GB ($24.00)</c:v>
                 </c:pt>
                 <c:pt idx="6">
+                  <c:v>EU BloomHost Performance+ 8GB ($22.00)</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>EU BloomHost Performance 8GB ($16.00)</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>NA Birdflop Premium 4GB ($12.00)</c:v>
                 </c:pt>
-                <c:pt idx="7">
-                  <c:v>EU Volcano Hosting Premium 4GB ($9.51)</c:v>
-                </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
+                  <c:v>EU Volcano Hosting Premium 4GB ($9.43)</c:v>
+                </c:pt>
+                <c:pt idx="10">
                   <c:v>NA PebbleHost Premium 4GB ($9.00)</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="11">
                   <c:v>EU Birdflop Premium 4GB ($8.00)</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="12">
                   <c:v>NA EnviroMC Budget 4GB ($4.00)</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="13">
                   <c:v>NA PebbleHost Budget 3GB ($3.00)</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="14">
                   <c:v>NA Daemex Beta 4GB ($0.00)</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="15">
                   <c:v>GLOBAL Baseline G4400 4GB (N/A)</c:v>
                 </c:pt>
               </c:strCache>
@@ -1088,10 +1136,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$F$3:$F$16</c:f>
+              <c:f>Sheet1!$F$3:$F$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="14"/>
+                <c:ptCount val="16"/>
                 <c:pt idx="0">
                   <c:v>105</c:v>
                 </c:pt>
@@ -1111,27 +1159,33 @@
                   <c:v>311</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>196</c:v>
+                  <c:v>128</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>123</c:v>
                 </c:pt>
                 <c:pt idx="8">
+                  <c:v>196</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>123</c:v>
+                </c:pt>
+                <c:pt idx="10">
                   <c:v>45</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="11">
                   <c:v>197</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="12">
                   <c:v>102</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="13">
                   <c:v>58</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="14">
                   <c:v>82</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="15">
                   <c:v>100</c:v>
                 </c:pt>
               </c:numCache>
@@ -1290,7 +1344,9 @@
         <c:spPr>
           <a:noFill/>
           <a:ln>
-            <a:noFill/>
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
           </a:ln>
           <a:effectLst/>
         </c:spPr>
@@ -2459,14 +2515,14 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>190499</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
       <xdr:colOff>600075</xdr:colOff>
       <xdr:row>36</xdr:row>
-      <xdr:rowOff>1</xdr:rowOff>
+      <xdr:rowOff>142874</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2495,14 +2551,14 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>35</xdr:row>
-      <xdr:rowOff>185737</xdr:rowOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>128586</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>52</xdr:row>
-      <xdr:rowOff>1</xdr:rowOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>190499</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2827,10 +2883,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{049E8E79-07BD-45DF-9A6A-257E2C4C3481}">
-  <dimension ref="A1:G16"/>
+  <dimension ref="A1:G18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="N44" sqref="N44"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="T32" sqref="T32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2974,7 +3030,7 @@
         <v>36.159999999999997</v>
       </c>
       <c r="E8" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="F8">
         <v>311</v>
@@ -2985,7 +3041,7 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B9">
         <v>196</v>
@@ -2994,10 +3050,10 @@
         <v>0</v>
       </c>
       <c r="E9" t="s">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="F9">
-        <v>196</v>
+        <v>128</v>
       </c>
       <c r="G9">
         <v>0</v>
@@ -3005,16 +3061,16 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B10">
-        <v>68</v>
+        <v>210</v>
       </c>
       <c r="C10">
         <v>0</v>
       </c>
       <c r="E10" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="F10">
         <v>123</v>
@@ -3025,19 +3081,19 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>6</v>
+        <v>21</v>
       </c>
       <c r="B11">
-        <v>49</v>
+        <v>137</v>
       </c>
       <c r="C11">
         <v>0</v>
       </c>
       <c r="E11" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="F11">
-        <v>45</v>
+        <v>196</v>
       </c>
       <c r="G11">
         <v>0</v>
@@ -3045,19 +3101,19 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="B12">
-        <v>176</v>
+        <v>68</v>
       </c>
       <c r="C12">
         <v>0</v>
       </c>
       <c r="E12" t="s">
-        <v>8</v>
+        <v>23</v>
       </c>
       <c r="F12">
-        <v>197</v>
+        <v>123</v>
       </c>
       <c r="G12">
         <v>0</v>
@@ -3065,19 +3121,19 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>21</v>
+        <v>6</v>
       </c>
       <c r="B13">
-        <v>115</v>
+        <v>49</v>
       </c>
       <c r="C13">
         <v>0</v>
       </c>
       <c r="E13" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F13">
-        <v>102</v>
+        <v>45</v>
       </c>
       <c r="G13">
         <v>0</v>
@@ -3085,19 +3141,19 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B14">
-        <v>66</v>
+        <v>176</v>
       </c>
       <c r="C14">
         <v>0</v>
       </c>
       <c r="E14" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="F14">
-        <v>58</v>
+        <v>197</v>
       </c>
       <c r="G14">
         <v>0</v>
@@ -3105,19 +3161,19 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="B15">
-        <v>46</v>
+        <v>115</v>
       </c>
       <c r="C15">
         <v>0</v>
       </c>
       <c r="E15" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="F15">
-        <v>82</v>
+        <v>102</v>
       </c>
       <c r="G15">
         <v>0</v>
@@ -3125,21 +3181,61 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>7</v>
+      </c>
+      <c r="B16">
+        <v>66</v>
+      </c>
+      <c r="C16">
+        <v>0</v>
+      </c>
+      <c r="E16" t="s">
+        <v>10</v>
+      </c>
+      <c r="F16">
+        <v>58</v>
+      </c>
+      <c r="G16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>16</v>
+      </c>
+      <c r="B17">
+        <v>46</v>
+      </c>
+      <c r="C17">
+        <v>0</v>
+      </c>
+      <c r="E17" t="s">
+        <v>16</v>
+      </c>
+      <c r="F17">
+        <v>82</v>
+      </c>
+      <c r="G17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>5</v>
       </c>
-      <c r="B16">
+      <c r="B18">
         <v>100</v>
       </c>
-      <c r="C16">
+      <c r="C18">
         <v>4.0599999999999996</v>
       </c>
-      <c r="E16" t="s">
+      <c r="E18" t="s">
         <v>5</v>
       </c>
-      <c r="F16">
+      <c r="F18">
         <v>100</v>
       </c>
-      <c r="G16">
+      <c r="G18">
         <v>3.27</v>
       </c>
     </row>

</xml_diff>